<commit_message>
Atualizando tabela resumo com 4-4-2 para jogador virtual que escolhe time de maior score
</commit_message>
<xml_diff>
--- a/analises_dos_dados_preliminares/Tabela Resumo - Scores Maximos para Referencia - Base Completa.xlsx
+++ b/analises_dos_dados_preliminares/Tabela Resumo - Scores Maximos para Referencia - Base Completa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dpcrj\OneDrive\Área de Trabalho\Faculdade\TCC_code\sportsAnalytics\analises_dos_dados_preliminares\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C69B9C9-E6A9-4C29-A54E-875C9699E212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7702EF-3AA9-4FAF-9C1D-E61EA9BD5B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E9A74655-EF3A-4D07-BF81-EB4937CE87C6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Rodadas</t>
   </si>
@@ -69,12 +69,24 @@
   <si>
     <t>SCORE MAX do Time (por rodada):</t>
   </si>
+  <si>
+    <t>SCORE 4-4-2 - Time de Maior Score (media)</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>MEDIA 4-4-2 - Time de Maior Score (media)</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +120,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -208,10 +227,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -252,9 +272,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="38">
     <dxf>
@@ -947,21 +974,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A35BF769-1BBC-45BD-B8DC-578ECD26FCB5}">
-  <dimension ref="B1:AO17"/>
+  <dimension ref="A1:AQ17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AO11" sqref="AO11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="5" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="31" max="31" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:41" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:43" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1003,7 +1030,7 @@
       <c r="AM1" s="14"/>
       <c r="AN1" s="15"/>
     </row>
-    <row r="2" spans="2:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
@@ -1125,7 +1152,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1248,7 +1278,7 @@
         <v>6926.36</v>
       </c>
     </row>
-    <row r="4" spans="2:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1371,7 +1401,7 @@
         <v>6666.2599999999966</v>
       </c>
     </row>
-    <row r="5" spans="2:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1494,7 +1524,10 @@
         <v>6780.3599999999988</v>
       </c>
     </row>
-    <row r="6" spans="2:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1617,7 +1650,7 @@
         <v>7006.36</v>
       </c>
     </row>
-    <row r="7" spans="2:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1740,7 +1773,10 @@
         <v>6733.3600000000006</v>
       </c>
     </row>
-    <row r="8" spans="2:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1863,7 +1899,7 @@
         <v>6871.4599999999991</v>
       </c>
     </row>
-    <row r="9" spans="2:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1986,11 +2022,11 @@
         <v>6711.2599999999993</v>
       </c>
     </row>
-    <row r="10" spans="2:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="AO10" s="9"/>
     </row>
-    <row r="11" spans="2:41" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:43" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
@@ -2147,12 +2183,276 @@
         <v>197.69999999999996</v>
       </c>
       <c r="AO11" s="6">
-        <f t="shared" ref="AO4:AO11" si="2">SUM(C11:AN11)</f>
+        <f t="shared" ref="AO11:AO16" si="2">SUM(C11:AN11)</f>
         <v>7030.6600000000008</v>
       </c>
     </row>
-    <row r="12" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
+      <c r="AO12" s="6"/>
+    </row>
+    <row r="13" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AO13" s="6"/>
+    </row>
+    <row r="14" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AO14" s="6"/>
+      <c r="AQ14" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:43" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B15" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="5">
+        <v>133.18</v>
+      </c>
+      <c r="D15" s="5">
+        <v>148.18999999999997</v>
+      </c>
+      <c r="E15" s="5">
+        <v>109.22</v>
+      </c>
+      <c r="F15" s="5">
+        <v>122.12999999999998</v>
+      </c>
+      <c r="G15" s="5">
+        <v>111.28</v>
+      </c>
+      <c r="H15" s="5">
+        <v>134.83000000000001</v>
+      </c>
+      <c r="I15" s="5">
+        <v>89.439999999999984</v>
+      </c>
+      <c r="J15" s="5">
+        <v>114.54</v>
+      </c>
+      <c r="K15" s="5">
+        <v>77.320000000000007</v>
+      </c>
+      <c r="L15" s="5">
+        <v>127.05000000000001</v>
+      </c>
+      <c r="M15" s="5">
+        <v>84.66</v>
+      </c>
+      <c r="N15" s="5">
+        <v>82.31</v>
+      </c>
+      <c r="O15" s="5">
+        <v>76.839999999999989</v>
+      </c>
+      <c r="P15" s="5">
+        <v>85.589999999999989</v>
+      </c>
+      <c r="Q15" s="5">
+        <v>75.48</v>
+      </c>
+      <c r="R15" s="5">
+        <v>79.669999999999987</v>
+      </c>
+      <c r="S15" s="5">
+        <v>92.240000000000023</v>
+      </c>
+      <c r="T15" s="5">
+        <v>84.89</v>
+      </c>
+      <c r="U15" s="5">
+        <v>93.529999999999987</v>
+      </c>
+      <c r="V15" s="5">
+        <v>57.589999999999996</v>
+      </c>
+      <c r="W15" s="5">
+        <v>52.059999999999995</v>
+      </c>
+      <c r="X15" s="5">
+        <v>47.4</v>
+      </c>
+      <c r="Y15" s="5">
+        <v>50.15</v>
+      </c>
+      <c r="Z15" s="5">
+        <v>67.69</v>
+      </c>
+      <c r="AA15" s="5">
+        <v>82.29</v>
+      </c>
+      <c r="AB15" s="5">
+        <v>54.550000000000011</v>
+      </c>
+      <c r="AC15" s="5">
+        <v>40.019999999999996</v>
+      </c>
+      <c r="AD15" s="5">
+        <v>49.239999999999995</v>
+      </c>
+      <c r="AE15" s="5">
+        <v>28.64</v>
+      </c>
+      <c r="AF15" s="5">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="AG15" s="5">
+        <v>70.88</v>
+      </c>
+      <c r="AH15" s="5">
+        <v>39.250000000000007</v>
+      </c>
+      <c r="AI15" s="5">
+        <v>30.419999999999998</v>
+      </c>
+      <c r="AJ15" s="5">
+        <v>58.360000000000007</v>
+      </c>
+      <c r="AK15" s="5">
+        <v>53.960000000000008</v>
+      </c>
+      <c r="AL15" s="5">
+        <v>52.75</v>
+      </c>
+      <c r="AM15" s="5">
+        <v>120.16000000000003</v>
+      </c>
+      <c r="AN15" s="5">
+        <v>75.150000000000006</v>
+      </c>
+      <c r="AO15" s="6">
+        <f t="shared" si="2"/>
+        <v>2992.75</v>
+      </c>
+      <c r="AQ15" s="5">
+        <f>(AO15*100)/$AO$3</f>
+        <v>43.20812086001883</v>
+      </c>
+    </row>
+    <row r="16" spans="1:43" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B16" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="5">
+        <v>133.17999999999998</v>
+      </c>
+      <c r="D16" s="5">
+        <v>102.19</v>
+      </c>
+      <c r="E16" s="5">
+        <v>94.8</v>
+      </c>
+      <c r="F16" s="5">
+        <v>93.98</v>
+      </c>
+      <c r="G16" s="5">
+        <v>93.719999999999985</v>
+      </c>
+      <c r="H16" s="5">
+        <v>107.23000000000002</v>
+      </c>
+      <c r="I16" s="5">
+        <v>94.250000000000014</v>
+      </c>
+      <c r="J16" s="5">
+        <v>121.65</v>
+      </c>
+      <c r="K16" s="5">
+        <v>93.74</v>
+      </c>
+      <c r="L16" s="5">
+        <v>87.56</v>
+      </c>
+      <c r="M16" s="5">
+        <v>86.899999999999977</v>
+      </c>
+      <c r="N16" s="5">
+        <v>88.26</v>
+      </c>
+      <c r="O16" s="5">
+        <v>73.64</v>
+      </c>
+      <c r="P16" s="5">
+        <v>78.64</v>
+      </c>
+      <c r="Q16" s="5">
+        <v>83.72</v>
+      </c>
+      <c r="R16" s="5">
+        <v>75.08</v>
+      </c>
+      <c r="S16" s="5">
+        <v>73.239999999999995</v>
+      </c>
+      <c r="T16" s="5">
+        <v>87.77</v>
+      </c>
+      <c r="U16" s="5">
+        <v>84.850000000000009</v>
+      </c>
+      <c r="V16" s="5">
+        <v>72.36999999999999</v>
+      </c>
+      <c r="W16" s="5">
+        <v>66.58</v>
+      </c>
+      <c r="X16" s="5">
+        <v>73.680000000000007</v>
+      </c>
+      <c r="Y16" s="5">
+        <v>68.72999999999999</v>
+      </c>
+      <c r="Z16" s="5">
+        <v>66.63</v>
+      </c>
+      <c r="AA16" s="5">
+        <v>72.989999999999995</v>
+      </c>
+      <c r="AB16" s="5">
+        <v>70.95</v>
+      </c>
+      <c r="AC16" s="5">
+        <v>63.269999999999989</v>
+      </c>
+      <c r="AD16" s="5">
+        <v>63.810000000000009</v>
+      </c>
+      <c r="AE16" s="5">
+        <v>64.09</v>
+      </c>
+      <c r="AF16" s="5">
+        <v>64.44</v>
+      </c>
+      <c r="AG16" s="5">
+        <v>57.959999999999994</v>
+      </c>
+      <c r="AH16" s="5">
+        <v>57.04</v>
+      </c>
+      <c r="AI16" s="5">
+        <v>59.230000000000004</v>
+      </c>
+      <c r="AJ16" s="5">
+        <v>53.510000000000005</v>
+      </c>
+      <c r="AK16" s="5">
+        <v>56.47</v>
+      </c>
+      <c r="AL16" s="5">
+        <v>62.680000000000007</v>
+      </c>
+      <c r="AM16" s="5">
+        <v>77.55</v>
+      </c>
+      <c r="AN16" s="5">
+        <v>77.389999999999986</v>
+      </c>
+      <c r="AO16" s="6">
+        <f>SUM(C16:AN16)</f>
+        <v>3003.7699999999995</v>
+      </c>
+      <c r="AQ16" s="5">
+        <f>(AO16*100)/$AO$3</f>
+        <v>43.367223187937093</v>
+      </c>
     </row>
     <row r="17" spans="31:31" x14ac:dyDescent="0.25">
       <c r="AE17" s="8"/>

</xml_diff>

<commit_message>
Adicionando tabela com escolhas para o jogador com os maiores scores para o esquema tático 5-3-2
</commit_message>
<xml_diff>
--- a/analises_dos_dados_preliminares/Tabela Resumo - Scores Maximos para Referencia - Base Completa.xlsx
+++ b/analises_dos_dados_preliminares/Tabela Resumo - Scores Maximos para Referencia - Base Completa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dpcrj\OneDrive\Área de Trabalho\Faculdade\TCC_code\sportsAnalytics\analises_dos_dados_preliminares\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7702EF-3AA9-4FAF-9C1D-E61EA9BD5B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2B196F-B21A-45CB-BCA3-23A0B39FF721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E9A74655-EF3A-4D07-BF81-EB4937CE87C6}"/>
   </bookViews>
@@ -76,10 +76,10 @@
     <t>%</t>
   </si>
   <si>
-    <t>MEDIA 4-4-2 - Time de Maior Score (media)</t>
+    <t>*</t>
   </si>
   <si>
-    <t>*</t>
+    <t>SCORE 5-3-2 - Time de Maior Score (media)</t>
   </si>
 </sst>
 </file>
@@ -231,7 +231,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -263,6 +263,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -272,11 +278,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -977,7 +980,7 @@
   <dimension ref="A1:AQ17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,46 +992,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
-      <c r="AB1" s="14"/>
-      <c r="AC1" s="14"/>
-      <c r="AD1" s="14"/>
-      <c r="AE1" s="14"/>
-      <c r="AF1" s="14"/>
-      <c r="AG1" s="14"/>
-      <c r="AH1" s="14"/>
-      <c r="AI1" s="14"/>
-      <c r="AJ1" s="14"/>
-      <c r="AK1" s="14"/>
-      <c r="AL1" s="14"/>
-      <c r="AM1" s="14"/>
-      <c r="AN1" s="15"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="16"/>
+      <c r="AE1" s="16"/>
+      <c r="AF1" s="16"/>
+      <c r="AG1" s="16"/>
+      <c r="AH1" s="16"/>
+      <c r="AI1" s="16"/>
+      <c r="AJ1" s="16"/>
+      <c r="AK1" s="16"/>
+      <c r="AL1" s="16"/>
+      <c r="AM1" s="16"/>
+      <c r="AN1" s="17"/>
     </row>
     <row r="2" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
@@ -1154,7 +1157,7 @@
     </row>
     <row r="3" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
@@ -1526,7 +1529,7 @@
     </row>
     <row r="6" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
@@ -1775,7 +1778,7 @@
     </row>
     <row r="8" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
@@ -2196,12 +2199,12 @@
     </row>
     <row r="14" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AO14" s="6"/>
-      <c r="AQ14" s="17" t="s">
+      <c r="AQ14" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:43" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="5">
@@ -2322,136 +2325,136 @@
         <f t="shared" si="2"/>
         <v>2992.75</v>
       </c>
-      <c r="AQ15" s="5">
+      <c r="AQ15" s="18">
         <f>(AO15*100)/$AO$3</f>
         <v>43.20812086001883</v>
       </c>
     </row>
     <row r="16" spans="1:43" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B16" s="16" t="s">
-        <v>13</v>
+      <c r="B16" s="13" t="s">
+        <v>14</v>
       </c>
       <c r="C16" s="5">
-        <v>133.17999999999998</v>
+        <v>132.77999999999997</v>
       </c>
       <c r="D16" s="5">
-        <v>102.19</v>
+        <v>124.44</v>
       </c>
       <c r="E16" s="5">
-        <v>94.8</v>
+        <v>109.13000000000002</v>
       </c>
       <c r="F16" s="5">
-        <v>93.98</v>
+        <v>128.43</v>
       </c>
       <c r="G16" s="5">
-        <v>93.719999999999985</v>
+        <v>113.92999999999999</v>
       </c>
       <c r="H16" s="5">
-        <v>107.23000000000002</v>
+        <v>130.73000000000002</v>
       </c>
       <c r="I16" s="5">
-        <v>94.250000000000014</v>
+        <v>97.039999999999992</v>
       </c>
       <c r="J16" s="5">
-        <v>121.65</v>
+        <v>115.78000000000002</v>
       </c>
       <c r="K16" s="5">
-        <v>93.74</v>
+        <v>85.1</v>
       </c>
       <c r="L16" s="5">
-        <v>87.56</v>
+        <v>125.75000000000001</v>
       </c>
       <c r="M16" s="5">
-        <v>86.899999999999977</v>
+        <v>84.160000000000011</v>
       </c>
       <c r="N16" s="5">
-        <v>88.26</v>
+        <v>85.51</v>
       </c>
       <c r="O16" s="5">
-        <v>73.64</v>
+        <v>77.839999999999989</v>
       </c>
       <c r="P16" s="5">
-        <v>78.64</v>
+        <v>81.289999999999992</v>
       </c>
       <c r="Q16" s="5">
-        <v>83.72</v>
+        <v>67.7</v>
       </c>
       <c r="R16" s="5">
-        <v>75.08</v>
+        <v>89.12</v>
       </c>
       <c r="S16" s="5">
-        <v>73.239999999999995</v>
+        <v>85.990000000000009</v>
       </c>
       <c r="T16" s="5">
-        <v>87.77</v>
+        <v>93.09</v>
       </c>
       <c r="U16" s="5">
-        <v>84.850000000000009</v>
+        <v>80.930000000000007</v>
       </c>
       <c r="V16" s="5">
-        <v>72.36999999999999</v>
+        <v>40.590000000000003</v>
       </c>
       <c r="W16" s="5">
-        <v>66.58</v>
+        <v>37.36</v>
       </c>
       <c r="X16" s="5">
-        <v>73.680000000000007</v>
+        <v>59.3</v>
       </c>
       <c r="Y16" s="5">
-        <v>68.72999999999999</v>
+        <v>50.650000000000006</v>
       </c>
       <c r="Z16" s="5">
-        <v>66.63</v>
+        <v>75.489999999999995</v>
       </c>
       <c r="AA16" s="5">
-        <v>72.989999999999995</v>
+        <v>69.490000000000009</v>
       </c>
       <c r="AB16" s="5">
-        <v>70.95</v>
+        <v>51.45</v>
       </c>
       <c r="AC16" s="5">
-        <v>63.269999999999989</v>
+        <v>37.119999999999997</v>
       </c>
       <c r="AD16" s="5">
-        <v>63.810000000000009</v>
+        <v>48.74</v>
       </c>
       <c r="AE16" s="5">
-        <v>64.09</v>
+        <v>28.54</v>
       </c>
       <c r="AF16" s="5">
-        <v>64.44</v>
+        <v>45.599999999999994</v>
       </c>
       <c r="AG16" s="5">
-        <v>57.959999999999994</v>
+        <v>72.319999999999993</v>
       </c>
       <c r="AH16" s="5">
-        <v>57.04</v>
+        <v>42.65</v>
       </c>
       <c r="AI16" s="5">
-        <v>59.230000000000004</v>
+        <v>25.02</v>
       </c>
       <c r="AJ16" s="5">
-        <v>53.510000000000005</v>
+        <v>52.960000000000008</v>
       </c>
       <c r="AK16" s="5">
-        <v>56.47</v>
+        <v>55.16</v>
       </c>
       <c r="AL16" s="5">
-        <v>62.680000000000007</v>
+        <v>43.45</v>
       </c>
       <c r="AM16" s="5">
-        <v>77.55</v>
+        <v>108.56000000000003</v>
       </c>
       <c r="AN16" s="5">
-        <v>77.389999999999986</v>
+        <v>72.170000000000016</v>
       </c>
       <c r="AO16" s="6">
-        <f>SUM(C16:AN16)</f>
-        <v>3003.7699999999995</v>
-      </c>
-      <c r="AQ16" s="5">
-        <f>(AO16*100)/$AO$3</f>
-        <v>43.367223187937093</v>
+        <f t="shared" si="2"/>
+        <v>2925.3599999999992</v>
+      </c>
+      <c r="AQ16" s="18">
+        <f>(AO16*100)/$AO$8</f>
+        <v>42.572611933999468</v>
       </c>
     </row>
     <row r="17" spans="31:31" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adicionando esquema 4-3-3 para jogadores com maiores scores e atualizando tabela resumo
</commit_message>
<xml_diff>
--- a/analises_dos_dados_preliminares/Tabela Resumo - Scores Maximos para Referencia - Base Completa.xlsx
+++ b/analises_dos_dados_preliminares/Tabela Resumo - Scores Maximos para Referencia - Base Completa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dpcrj\OneDrive\Área de Trabalho\Faculdade\TCC_code\sportsAnalytics\analises_dos_dados_preliminares\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2B196F-B21A-45CB-BCA3-23A0B39FF721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB68444-FF80-4E55-85FE-E746B4FE0C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E9A74655-EF3A-4D07-BF81-EB4937CE87C6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Rodadas</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>SCORE 5-3-2 - Time de Maior Score (media)</t>
+  </si>
+  <si>
+    <t>SCORE 4-3-3 - Time de Maior Score (media)</t>
   </si>
 </sst>
 </file>
@@ -231,7 +234,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -250,7 +253,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -269,6 +271,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -277,9 +282,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -979,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A35BF769-1BBC-45BD-B8DC-578ECD26FCB5}">
   <dimension ref="A1:AQ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="AK16" sqref="AK16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,118 +1039,118 @@
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="9">
         <v>1</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="10">
         <v>2</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="10">
         <v>3</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="10">
         <v>4</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="10">
         <v>5</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="10">
         <v>6</v>
       </c>
-      <c r="I2" s="11">
+      <c r="I2" s="10">
         <v>7</v>
       </c>
-      <c r="J2" s="11">
+      <c r="J2" s="10">
         <v>8</v>
       </c>
-      <c r="K2" s="11">
+      <c r="K2" s="10">
         <v>9</v>
       </c>
-      <c r="L2" s="11">
+      <c r="L2" s="10">
         <v>10</v>
       </c>
-      <c r="M2" s="11">
+      <c r="M2" s="10">
         <v>11</v>
       </c>
-      <c r="N2" s="11">
+      <c r="N2" s="10">
         <v>12</v>
       </c>
-      <c r="O2" s="11">
+      <c r="O2" s="10">
         <v>13</v>
       </c>
-      <c r="P2" s="11">
+      <c r="P2" s="10">
         <v>14</v>
       </c>
-      <c r="Q2" s="11">
+      <c r="Q2" s="10">
         <v>15</v>
       </c>
-      <c r="R2" s="11">
+      <c r="R2" s="10">
         <v>16</v>
       </c>
-      <c r="S2" s="11">
+      <c r="S2" s="10">
         <v>17</v>
       </c>
-      <c r="T2" s="11">
+      <c r="T2" s="10">
         <v>18</v>
       </c>
-      <c r="U2" s="11">
+      <c r="U2" s="10">
         <v>19</v>
       </c>
-      <c r="V2" s="11">
+      <c r="V2" s="10">
         <v>20</v>
       </c>
-      <c r="W2" s="11">
+      <c r="W2" s="10">
         <v>21</v>
       </c>
-      <c r="X2" s="11">
+      <c r="X2" s="10">
         <v>22</v>
       </c>
-      <c r="Y2" s="11">
+      <c r="Y2" s="10">
         <v>23</v>
       </c>
-      <c r="Z2" s="11">
+      <c r="Z2" s="10">
         <v>24</v>
       </c>
-      <c r="AA2" s="11">
+      <c r="AA2" s="10">
         <v>25</v>
       </c>
-      <c r="AB2" s="11">
+      <c r="AB2" s="10">
         <v>26</v>
       </c>
-      <c r="AC2" s="11">
+      <c r="AC2" s="10">
         <v>27</v>
       </c>
-      <c r="AD2" s="11">
+      <c r="AD2" s="10">
         <v>28</v>
       </c>
-      <c r="AE2" s="11">
+      <c r="AE2" s="10">
         <v>29</v>
       </c>
-      <c r="AF2" s="11">
+      <c r="AF2" s="10">
         <v>30</v>
       </c>
-      <c r="AG2" s="11">
+      <c r="AG2" s="10">
         <v>31</v>
       </c>
-      <c r="AH2" s="11">
+      <c r="AH2" s="10">
         <v>32</v>
       </c>
-      <c r="AI2" s="11">
+      <c r="AI2" s="10">
         <v>33</v>
       </c>
-      <c r="AJ2" s="11">
+      <c r="AJ2" s="10">
         <v>34</v>
       </c>
-      <c r="AK2" s="11">
+      <c r="AK2" s="10">
         <v>35</v>
       </c>
-      <c r="AL2" s="11">
+      <c r="AL2" s="10">
         <v>36</v>
       </c>
-      <c r="AM2" s="11">
+      <c r="AM2" s="10">
         <v>37</v>
       </c>
-      <c r="AN2" s="12">
+      <c r="AN2" s="11">
         <v>38</v>
       </c>
       <c r="AO2" s="3" t="s">
@@ -1276,7 +1278,7 @@
       <c r="AN3">
         <v>193.49999999999997</v>
       </c>
-      <c r="AO3" s="9">
+      <c r="AO3" s="8">
         <f>SUM(C3:AN3)</f>
         <v>6926.36</v>
       </c>
@@ -1399,7 +1401,7 @@
       <c r="AN4">
         <v>185.89999999999995</v>
       </c>
-      <c r="AO4" s="9">
+      <c r="AO4" s="8">
         <f t="shared" ref="AO4:AO9" si="0">SUM(C4:AN4)</f>
         <v>6666.2599999999966</v>
       </c>
@@ -1522,7 +1524,7 @@
       <c r="AN5">
         <v>190.39999999999998</v>
       </c>
-      <c r="AO5" s="9">
+      <c r="AO5" s="8">
         <f t="shared" si="0"/>
         <v>6780.3599999999988</v>
       </c>
@@ -1648,7 +1650,7 @@
       <c r="AN6">
         <v>197.69999999999996</v>
       </c>
-      <c r="AO6" s="9">
+      <c r="AO6" s="8">
         <f t="shared" si="0"/>
         <v>7006.36</v>
       </c>
@@ -1771,7 +1773,7 @@
       <c r="AN7">
         <v>188.39999999999998</v>
       </c>
-      <c r="AO7" s="9">
+      <c r="AO7" s="8">
         <f t="shared" si="0"/>
         <v>6733.3600000000006</v>
       </c>
@@ -1897,7 +1899,7 @@
       <c r="AN8">
         <v>188.99999999999994</v>
       </c>
-      <c r="AO8" s="9">
+      <c r="AO8" s="8">
         <f t="shared" si="0"/>
         <v>6871.4599999999991</v>
       </c>
@@ -2020,14 +2022,14 @@
       <c r="AN9">
         <v>184.19999999999996</v>
       </c>
-      <c r="AO9" s="9">
+      <c r="AO9" s="8">
         <f t="shared" si="0"/>
         <v>6711.2599999999993</v>
       </c>
     </row>
     <row r="10" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
-      <c r="AO10" s="9"/>
+      <c r="AO10" s="8"/>
     </row>
     <row r="11" spans="1:43" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
@@ -2199,12 +2201,12 @@
     </row>
     <row r="14" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AO14" s="6"/>
-      <c r="AQ14" s="14" t="s">
+      <c r="AQ14" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:43" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="5">
@@ -2325,140 +2327,265 @@
         <f t="shared" si="2"/>
         <v>2992.75</v>
       </c>
-      <c r="AQ15" s="18">
+      <c r="AQ15" s="14">
         <f>(AO15*100)/$AO$3</f>
         <v>43.20812086001883</v>
       </c>
     </row>
     <row r="16" spans="1:43" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B16" s="13" t="s">
-        <v>14</v>
+      <c r="B16" s="12" t="s">
+        <v>15</v>
       </c>
       <c r="C16" s="5">
-        <v>132.77999999999997</v>
+        <v>133.57999999999998</v>
       </c>
       <c r="D16" s="5">
-        <v>124.44</v>
+        <v>148.14000000000001</v>
       </c>
       <c r="E16" s="5">
-        <v>109.13000000000002</v>
+        <v>110.25</v>
       </c>
       <c r="F16" s="5">
-        <v>128.43</v>
+        <v>130.72</v>
       </c>
       <c r="G16" s="5">
-        <v>113.92999999999999</v>
+        <v>117.98</v>
       </c>
       <c r="H16" s="5">
-        <v>130.73000000000002</v>
+        <v>136.13000000000002</v>
       </c>
       <c r="I16" s="5">
-        <v>97.039999999999992</v>
+        <v>95.14</v>
       </c>
       <c r="J16" s="5">
-        <v>115.78000000000002</v>
+        <v>115.84000000000002</v>
       </c>
       <c r="K16" s="5">
-        <v>85.1</v>
+        <v>101.12000000000002</v>
       </c>
       <c r="L16" s="5">
-        <v>125.75000000000001</v>
+        <v>132.85000000000002</v>
       </c>
       <c r="M16" s="5">
-        <v>84.160000000000011</v>
+        <v>85.26</v>
       </c>
       <c r="N16" s="5">
-        <v>85.51</v>
+        <v>74.81</v>
       </c>
       <c r="O16" s="5">
-        <v>77.839999999999989</v>
+        <v>78.64</v>
       </c>
       <c r="P16" s="5">
-        <v>81.289999999999992</v>
+        <v>85.99</v>
       </c>
       <c r="Q16" s="5">
-        <v>67.7</v>
+        <v>73.8</v>
       </c>
       <c r="R16" s="5">
-        <v>89.12</v>
+        <v>90.420000000000016</v>
       </c>
       <c r="S16" s="5">
-        <v>85.990000000000009</v>
+        <v>69.77000000000001</v>
       </c>
       <c r="T16" s="5">
-        <v>93.09</v>
+        <v>99.39</v>
       </c>
       <c r="U16" s="5">
-        <v>80.930000000000007</v>
+        <v>76.330000000000013</v>
       </c>
       <c r="V16" s="5">
-        <v>40.590000000000003</v>
+        <v>63.39</v>
       </c>
       <c r="W16" s="5">
-        <v>37.36</v>
+        <v>35.160000000000004</v>
       </c>
       <c r="X16" s="5">
-        <v>59.3</v>
+        <v>51.999999999999993</v>
       </c>
       <c r="Y16" s="5">
-        <v>50.650000000000006</v>
+        <v>50.25</v>
       </c>
       <c r="Z16" s="5">
-        <v>75.489999999999995</v>
+        <v>44.589999999999996</v>
       </c>
       <c r="AA16" s="5">
-        <v>69.490000000000009</v>
+        <v>70.290000000000006</v>
       </c>
       <c r="AB16" s="5">
-        <v>51.45</v>
+        <v>56.59</v>
       </c>
       <c r="AC16" s="5">
-        <v>37.119999999999997</v>
+        <v>37.92</v>
       </c>
       <c r="AD16" s="5">
-        <v>48.74</v>
+        <v>46.84</v>
       </c>
       <c r="AE16" s="5">
-        <v>28.54</v>
+        <v>26.740000000000002</v>
       </c>
       <c r="AF16" s="5">
-        <v>45.599999999999994</v>
+        <v>55.2</v>
       </c>
       <c r="AG16" s="5">
-        <v>72.319999999999993</v>
+        <v>74.62</v>
       </c>
       <c r="AH16" s="5">
-        <v>42.65</v>
+        <v>37.950000000000003</v>
       </c>
       <c r="AI16" s="5">
-        <v>25.02</v>
+        <v>37.359999999999992</v>
       </c>
       <c r="AJ16" s="5">
-        <v>52.960000000000008</v>
+        <v>62.160000000000004</v>
       </c>
       <c r="AK16" s="5">
-        <v>55.16</v>
+        <v>54.66</v>
       </c>
       <c r="AL16" s="5">
-        <v>43.45</v>
+        <v>57.550000000000004</v>
       </c>
       <c r="AM16" s="5">
-        <v>108.56000000000003</v>
+        <v>110.76000000000003</v>
       </c>
       <c r="AN16" s="5">
-        <v>72.170000000000016</v>
+        <v>88.350000000000009</v>
       </c>
       <c r="AO16" s="6">
         <f t="shared" si="2"/>
+        <v>3018.54</v>
+      </c>
+      <c r="AQ16" s="14">
+        <f>(AO16*100)/$AO$6</f>
+        <v>43.082856147842818</v>
+      </c>
+    </row>
+    <row r="17" spans="2:43" ht="45" x14ac:dyDescent="0.25">
+      <c r="B17" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="5">
+        <v>132.77999999999997</v>
+      </c>
+      <c r="D17" s="5">
+        <v>124.44</v>
+      </c>
+      <c r="E17" s="5">
+        <v>109.13000000000002</v>
+      </c>
+      <c r="F17" s="5">
+        <v>128.43</v>
+      </c>
+      <c r="G17" s="5">
+        <v>113.92999999999999</v>
+      </c>
+      <c r="H17" s="5">
+        <v>130.73000000000002</v>
+      </c>
+      <c r="I17" s="5">
+        <v>97.039999999999992</v>
+      </c>
+      <c r="J17" s="5">
+        <v>115.78000000000002</v>
+      </c>
+      <c r="K17" s="5">
+        <v>85.1</v>
+      </c>
+      <c r="L17" s="5">
+        <v>125.75000000000001</v>
+      </c>
+      <c r="M17" s="5">
+        <v>84.160000000000011</v>
+      </c>
+      <c r="N17" s="5">
+        <v>85.51</v>
+      </c>
+      <c r="O17" s="5">
+        <v>77.839999999999989</v>
+      </c>
+      <c r="P17" s="5">
+        <v>81.289999999999992</v>
+      </c>
+      <c r="Q17" s="5">
+        <v>67.7</v>
+      </c>
+      <c r="R17" s="5">
+        <v>89.12</v>
+      </c>
+      <c r="S17" s="5">
+        <v>85.990000000000009</v>
+      </c>
+      <c r="T17" s="5">
+        <v>93.09</v>
+      </c>
+      <c r="U17" s="5">
+        <v>80.930000000000007</v>
+      </c>
+      <c r="V17" s="5">
+        <v>40.590000000000003</v>
+      </c>
+      <c r="W17" s="5">
+        <v>37.36</v>
+      </c>
+      <c r="X17" s="5">
+        <v>59.3</v>
+      </c>
+      <c r="Y17" s="5">
+        <v>50.650000000000006</v>
+      </c>
+      <c r="Z17" s="5">
+        <v>75.489999999999995</v>
+      </c>
+      <c r="AA17" s="5">
+        <v>69.490000000000009</v>
+      </c>
+      <c r="AB17" s="5">
+        <v>51.45</v>
+      </c>
+      <c r="AC17" s="5">
+        <v>37.119999999999997</v>
+      </c>
+      <c r="AD17" s="5">
+        <v>48.74</v>
+      </c>
+      <c r="AE17" s="5">
+        <v>28.54</v>
+      </c>
+      <c r="AF17" s="5">
+        <v>45.599999999999994</v>
+      </c>
+      <c r="AG17" s="5">
+        <v>72.319999999999993</v>
+      </c>
+      <c r="AH17" s="5">
+        <v>42.65</v>
+      </c>
+      <c r="AI17" s="5">
+        <v>25.02</v>
+      </c>
+      <c r="AJ17" s="5">
+        <v>52.960000000000008</v>
+      </c>
+      <c r="AK17" s="5">
+        <v>55.16</v>
+      </c>
+      <c r="AL17" s="5">
+        <v>43.45</v>
+      </c>
+      <c r="AM17" s="5">
+        <v>108.56000000000003</v>
+      </c>
+      <c r="AN17" s="5">
+        <v>72.170000000000016</v>
+      </c>
+      <c r="AO17" s="6">
+        <f>SUM(C17:AN17)</f>
         <v>2925.3599999999992</v>
       </c>
-      <c r="AQ16" s="18">
-        <f>(AO16*100)/$AO$8</f>
+      <c r="AP17" s="5"/>
+      <c r="AQ17" s="14">
+        <f>(AO17*100)/$AO$8</f>
         <v>42.572611933999468</v>
       </c>
-    </row>
-    <row r="17" spans="31:31" x14ac:dyDescent="0.25">
-      <c r="AE17" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>